<commit_message>
chore(lesson-plan): modified backend plan structure feat(material): added Git & GitHub material PDF
</commit_message>
<xml_diff>
--- a/Lesson_Plan.xlsx
+++ b/Lesson_Plan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="226">
   <si>
     <t>Hour</t>
   </si>
@@ -662,252 +662,15 @@
     <t>Apply full MongoDB workflow and test readiness</t>
   </si>
   <si>
-    <t>Node.js + Express + Mongosh</t>
-  </si>
-  <si>
-    <t>Node.js Intro + npm Scripts</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Node.js overview, environment setup, npm, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>package.json</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, scripts</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Install Node.js, initialize project, basic scripts (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>start</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, etc)</t>
-    </r>
-  </si>
-  <si>
-    <t>Understand Node.js setup and project initialization</t>
-  </si>
-  <si>
-    <t>Express Server Basics</t>
-  </si>
-  <si>
-    <t>Installing Express, basic server creation, route structure</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create "Hello World" app, use </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>app.get()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> &amp; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>app.post()</t>
-    </r>
-  </si>
-  <si>
-    <t>Build a simple server and handle GET/POST routes</t>
-  </si>
-  <si>
     <t>Middleware in Express</t>
   </si>
   <si>
-    <t>Built-in and custom middleware, body parsing, logging</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Add </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>express.json()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, logger middleware</t>
-    </r>
-  </si>
-  <si>
-    <t>Process incoming requests/responses effectively</t>
-  </si>
-  <si>
-    <t>MongoDB + Mongoose Setup</t>
-  </si>
-  <si>
     <t>Install Mongoose, connect to MongoDB Atlas/local</t>
   </si>
   <si>
-    <t>Connect Express app to MongoDB with Mongoose</t>
-  </si>
-  <si>
-    <t>Integrate MongoDB into Node.js project</t>
-  </si>
-  <si>
-    <t>Schema &amp; Model Definition</t>
-  </si>
-  <si>
-    <t>Define Mongoose schemas, models, data validation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create sample schema and model (e.g., </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial Unicode MS"/>
-      </rPr>
-      <t>Student</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Create data structure and ensure validation</t>
-  </si>
-  <si>
-    <t>CRUD API Routes</t>
-  </si>
-  <si>
-    <t>Implement API endpoints using Express + Mongoose</t>
-  </si>
-  <si>
-    <t>Build Create, Read, Update, Delete routes</t>
-  </si>
-  <si>
-    <t>Perform full CRUD operations via API</t>
-  </si>
-  <si>
-    <t>Testing API with Postman</t>
-  </si>
-  <si>
-    <t>Test endpoints, status codes, request bodies</t>
-  </si>
-  <si>
-    <t>Test all routes in Postman/browser</t>
-  </si>
-  <si>
-    <t>Debug and validate full API flow</t>
-  </si>
-  <si>
-    <t>Mini Project Scaffold</t>
-  </si>
-  <si>
-    <t>Combine all concepts in a mini project (e.g., Student/Task management API)</t>
-  </si>
-  <si>
-    <t>Scaffold project with routes, schema, DB, testing</t>
-  </si>
-  <si>
-    <t>Apply all concepts to build a complete RESTful API</t>
-  </si>
-  <si>
     <t>REST API Design + Postman</t>
   </si>
   <si>
-    <t>REST Concepts &amp; API Testing with Postman</t>
-  </si>
-  <si>
-    <t>REST principles, HTTP methods (GET, POST, PUT, DELETE), Postman setup &amp; testing basics</t>
-  </si>
-  <si>
-    <t>Map HTTP verbs to CRUD, test GET &amp; POST in Postman</t>
-  </si>
-  <si>
-    <t>Understand REST API design and interact with APIs via Postman</t>
-  </si>
-  <si>
-    <t>URI Design, CRUD Testing &amp; Response Codes</t>
-  </si>
-  <si>
-    <t>Endpoint naming, URI structure, PUT/DELETE testing, response formatting, status codes</t>
-  </si>
-  <si>
-    <t>Design URIs, perform full CRUD testing, use correct status codes</t>
-  </si>
-  <si>
-    <t>Create scalable endpoints and test all CRUD ops with proper feedback</t>
-  </si>
-  <si>
-    <t>Validation, Error Handling &amp; Code Structure</t>
-  </si>
-  <si>
-    <t>Express Validator, error handling middleware, routes/controllers separation</t>
-  </si>
-  <si>
-    <t>Add validation, implement error handlers, modularize code</t>
-  </si>
-  <si>
-    <t>Build secure, modular, and production-ready API structure</t>
-  </si>
-  <si>
     <t>HTML</t>
   </si>
   <si>
@@ -2082,6 +1845,265 @@
   </si>
   <si>
     <t>Not Completed</t>
+  </si>
+  <si>
+    <t>Node.js + Express + MongoDB</t>
+  </si>
+  <si>
+    <t>Node.js Intro, npm &amp; Scripts + Express App &amp; Routes</t>
+  </si>
+  <si>
+    <t>Node.js basics, REPL, npm init, install Express, define routes</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Init project, create server, build </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/hello</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/user/:id</t>
+    </r>
+  </si>
+  <si>
+    <t>Understand Node runtime and build basic Express server</t>
+  </si>
+  <si>
+    <t>Built-in/custom middleware, next(), logger, body-parser</t>
+  </si>
+  <si>
+    <t>Add logger &amp; body-parser middleware</t>
+  </si>
+  <si>
+    <t>Understand middleware layering and flow</t>
+  </si>
+  <si>
+    <t>Mongoose Setup &amp; DB Connection</t>
+  </si>
+  <si>
+    <t>Connect app to MongoDB</t>
+  </si>
+  <si>
+    <t>Set up DB connection using Mongoose</t>
+  </si>
+  <si>
+    <t>MongoDB + Mongoose CRUD</t>
+  </si>
+  <si>
+    <t>Define Schema &amp; Models</t>
+  </si>
+  <si>
+    <t>Schema types, validation, timestamps, methods</t>
+  </si>
+  <si>
+    <t>Build User and Product models</t>
+  </si>
+  <si>
+    <t>Define and validate MongoDB documents</t>
+  </si>
+  <si>
+    <t>CRUD Routes &amp; DB Ops + API Testing with Postman</t>
+  </si>
+  <si>
+    <t>CRUD operations (find, create, update, delete), Postman testing</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Build </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/products</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> routes, test CRUD in Postman</t>
+    </r>
+  </si>
+  <si>
+    <t>Perform DB ops and test API endpoints</t>
+  </si>
+  <si>
+    <t>REST Design &amp; Endpoints + Status Codes &amp; Input Validation</t>
+  </si>
+  <si>
+    <t>REST principles, naming, status codes, express-validator</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refactor URIs, add validation to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/register</t>
+    </r>
+  </si>
+  <si>
+    <t>Design clean REST APIs with validation</t>
+  </si>
+  <si>
+    <t>Error Handling &amp; Resilience + Project Structure</t>
+  </si>
+  <si>
+    <t>Try/catch, central error handler, modular structure</t>
+  </si>
+  <si>
+    <t>Break API, organize routes/controllers</t>
+  </si>
+  <si>
+    <t>Build stable, maintainable API structure</t>
+  </si>
+  <si>
+    <t>Authentication &amp; Integration</t>
+  </si>
+  <si>
+    <t>User Auth – Register/Login + JWT Token Authentication</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hashing, login logic, JWT creation, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>verifyToken</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/register</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, protect </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/dashboard</t>
+    </r>
+  </si>
+  <si>
+    <t>Add authentication and route protection</t>
+  </si>
+  <si>
+    <t>Auth Middleware &amp; Access</t>
+  </si>
+  <si>
+    <t>Middleware flow, access control logic</t>
+  </si>
+  <si>
+    <t>Block unauthorized users from routes</t>
+  </si>
+  <si>
+    <t>Restrict access using JWT</t>
+  </si>
+  <si>
+    <t>Final Project – Setup + Logic</t>
+  </si>
+  <si>
+    <t>Scaffold secure backend, product/user API logic, validation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement CRUD with auth for </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>/products</t>
+    </r>
+  </si>
+  <si>
+    <t>Apply full backend flow in real-world setup</t>
+  </si>
+  <si>
+    <t>Final Project – Security + Testing &amp; Wrap-up</t>
+  </si>
+  <si>
+    <t>Secure endpoints, Postman testing, deploy to Render</t>
+  </si>
+  <si>
+    <t>Final testing, deploy live</t>
+  </si>
+  <si>
+    <t>Secure and deploy functional backend API</t>
   </si>
 </sst>
 </file>
@@ -2130,7 +2152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2166,11 +2188,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2200,39 +2225,6 @@
           <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2296,13 +2288,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2315,6 +2301,15 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2333,28 +2328,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="19" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G51"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Hour" dataDxfId="12"/>
+    <tableColumn id="1" name="Hour" dataDxfId="14"/>
     <tableColumn id="2" name="Category" dataDxfId="13"/>
-    <tableColumn id="3" name="Topic" dataDxfId="18"/>
-    <tableColumn id="4" name="Subtopics Covered" dataDxfId="17"/>
-    <tableColumn id="5" name="Hands-on Activity" dataDxfId="16"/>
-    <tableColumn id="6" name="Learning Outcome" dataDxfId="15"/>
-    <tableColumn id="7" name="STATUS" dataDxfId="6"/>
+    <tableColumn id="3" name="Topic" dataDxfId="12"/>
+    <tableColumn id="4" name="Subtopics Covered" dataDxfId="11"/>
+    <tableColumn id="5" name="Hands-on Activity" dataDxfId="10"/>
+    <tableColumn id="6" name="Learning Outcome" dataDxfId="9"/>
+    <tableColumn id="7" name="STATUS" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5" displayName="Table5" ref="A1:C11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:C11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5" displayName="Table5" ref="A1:C13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:C13"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="WEB STACK" dataDxfId="9"/>
-    <tableColumn id="3" name="TOPIC" dataDxfId="8"/>
-    <tableColumn id="4" name="CRASH COURSE" dataDxfId="7"/>
+    <tableColumn id="2" name="WEB STACK" dataDxfId="5"/>
+    <tableColumn id="3" name="TOPIC" dataDxfId="4"/>
+    <tableColumn id="4" name="CRASH COURSE" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2625,9 +2620,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2657,7 +2650,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1">
@@ -2680,10 +2673,10 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1">
@@ -2706,10 +2699,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="I3" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1">
@@ -2732,10 +2725,10 @@
         <v>18</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="I4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1">
@@ -2758,7 +2751,7 @@
         <v>23</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1">
@@ -2781,7 +2774,7 @@
         <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1">
@@ -2804,7 +2797,7 @@
         <v>31</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1">
@@ -2827,7 +2820,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1">
@@ -2850,7 +2843,7 @@
         <v>39</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1">
@@ -2873,7 +2866,7 @@
         <v>43</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1">
@@ -2896,7 +2889,7 @@
         <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1">
@@ -2919,7 +2912,7 @@
         <v>51</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1">
@@ -2942,260 +2935,260 @@
         <v>55</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>60</v>
+      <c r="B14" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>185</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>64</v>
+      <c r="D15" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>68</v>
+      <c r="B16" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>191</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>72</v>
+      <c r="B17" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>76</v>
+      <c r="B18" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>200</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>80</v>
+      <c r="B19" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>84</v>
+      <c r="B20" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>208</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" customHeight="1">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>88</v>
+      <c r="B21" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>213</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>93</v>
+      <c r="B22" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>217</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" customHeight="1">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>97</v>
+      <c r="B23" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>221</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" customHeight="1">
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>101</v>
+      <c r="B24" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" customHeight="1">
@@ -3203,22 +3196,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>104</v>
+        <v>61</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>105</v>
+        <v>62</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>106</v>
+        <v>63</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" customHeight="1">
@@ -3226,22 +3219,22 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>102</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>109</v>
+        <v>66</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" customHeight="1">
@@ -3249,22 +3242,22 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" customHeight="1">
@@ -3272,22 +3265,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="30" customHeight="1">
@@ -3295,22 +3288,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" customHeight="1">
@@ -3318,22 +3311,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" customHeight="1">
@@ -3341,22 +3334,22 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30" customHeight="1">
@@ -3364,22 +3357,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" customHeight="1">
@@ -3387,22 +3380,22 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" customHeight="1">
@@ -3410,22 +3403,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" customHeight="1">
@@ -3433,22 +3426,22 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="30" customHeight="1">
@@ -3456,22 +3449,22 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" customHeight="1">
@@ -3479,22 +3472,22 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1">
@@ -3502,22 +3495,22 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1">
@@ -3525,22 +3518,22 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="30" customHeight="1">
@@ -3548,22 +3541,22 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" customHeight="1">
@@ -3571,22 +3564,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" customHeight="1">
@@ -3594,22 +3587,22 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" customHeight="1">
@@ -3617,22 +3610,22 @@
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" customHeight="1">
@@ -3640,22 +3633,22 @@
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>181</v>
+        <v>138</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>182</v>
+        <v>139</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>183</v>
+        <v>140</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>184</v>
+        <v>141</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" customHeight="1">
@@ -3663,22 +3656,22 @@
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>199</v>
+        <v>156</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>200</v>
+        <v>157</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="30" customHeight="1">
@@ -3686,22 +3679,22 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30" customHeight="1">
@@ -3709,22 +3702,22 @@
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>185</v>
+        <v>142</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>188</v>
+        <v>145</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="30" customHeight="1">
@@ -3732,22 +3725,22 @@
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>189</v>
+        <v>146</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>190</v>
+        <v>147</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>191</v>
+        <v>148</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>192</v>
+        <v>149</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" customHeight="1">
@@ -3755,22 +3748,22 @@
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>196</v>
+        <v>153</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" customHeight="1">
@@ -3778,22 +3771,22 @@
         <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>202</v>
+        <v>159</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>204</v>
+        <v>161</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" customHeight="1">
@@ -3801,34 +3794,34 @@
         <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>205</v>
+        <v>162</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Completed"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Partially Completed"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Not Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"Partially Completed"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -3849,10 +3842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3864,21 +3857,21 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="19.95" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>214</v>
+        <v>171</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>215</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.95" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="C2" s="9">
         <f>COUNTIF('MERN Stack'!B:B, "Git and GitHub")</f>
@@ -3898,75 +3891,95 @@
     <row r="4" spans="1:3" ht="19.95" customHeight="1">
       <c r="A4" s="8"/>
       <c r="B4" s="10" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="C4" s="9">
-        <f>COUNTIF('MERN Stack'!B:B, "Node.js + Express + Mongosh")</f>
-        <v>8</v>
+        <f>COUNTIF('MERN Stack'!B:B, "Node.js + Express + MongoDB")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.95" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="10" t="s">
-        <v>89</v>
+        <v>192</v>
       </c>
       <c r="C5" s="9">
-        <f>COUNTIF('MERN Stack'!B:B, "REST API Design + Postman")</f>
-        <v>3</v>
+        <f>COUNTIF('MERN Stack'!B:B, "MongoDB + Mongoose CRUD")</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.95" customHeight="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="8" t="s">
-        <v>102</v>
+      <c r="B6" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="9">
-        <f>COUNTIF('MERN Stack'!B:B, "HTML")</f>
+        <f>COUNTIF('MERN Stack'!B:B, "REST API Design + Postman")</f>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.95" customHeight="1">
       <c r="A7" s="8"/>
-      <c r="B7" s="8" t="s">
-        <v>111</v>
+      <c r="B7" s="10" t="s">
+        <v>209</v>
       </c>
       <c r="C7" s="9">
-        <f>COUNTIF('MERN Stack'!B:B, "CSS")</f>
+        <f>COUNTIF('MERN Stack'!B:B, "Authentication &amp; Integration")</f>
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.95" customHeight="1">
       <c r="A8" s="8"/>
       <c r="B8" s="8" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
       <c r="C8" s="9">
+        <f>COUNTIF('MERN Stack'!B:B, "HTML")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.95" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="9">
+        <f>COUNTIF('MERN Stack'!B:B, "CSS")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.95" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="9">
         <f>COUNTIF('MERN Stack'!B:B, "JavaScript")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="9">
+    <row r="11" spans="1:3" ht="19.95" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="9">
         <f>COUNTIF('MERN Stack'!B:B, "React and Rest API integration")</f>
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="9"/>
-    </row>
-    <row r="11" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="9">
-        <f>SUM(C2:C10)</f>
+    <row r="12" spans="1:3" ht="19.95" customHeight="1">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.95" customHeight="1">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="9">
+        <f>SUM(C2:C12)</f>
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore(lesson-plan): reordered flow to place HTML, CSS, JS before backend feat(material): added Node.js + Express + Mongoose PDF
</commit_message>
<xml_diff>
--- a/Lesson_Plan.xlsx
+++ b/Lesson_Plan.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD255669-36C2-44D1-9CF1-4A49B2059DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MERN Stack" sheetId="1" r:id="rId1"/>
     <sheet name="Lesson Plan Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2109,7 +2110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -2152,7 +2153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2169,23 +2170,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2328,28 +2319,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:G51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G51" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:G51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Hour" dataDxfId="14"/>
-    <tableColumn id="2" name="Category" dataDxfId="13"/>
-    <tableColumn id="3" name="Topic" dataDxfId="12"/>
-    <tableColumn id="4" name="Subtopics Covered" dataDxfId="11"/>
-    <tableColumn id="5" name="Hands-on Activity" dataDxfId="10"/>
-    <tableColumn id="6" name="Learning Outcome" dataDxfId="9"/>
-    <tableColumn id="7" name="STATUS" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Hour" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Category" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Topic" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Subtopics Covered" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Hands-on Activity" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Learning Outcome" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="STATUS" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table5" displayName="Table5" ref="A1:C13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:C13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table5" displayName="Table5" ref="A1:C13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:C13" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="2" name="WEB STACK" dataDxfId="5"/>
-    <tableColumn id="3" name="TOPIC" dataDxfId="4"/>
-    <tableColumn id="4" name="CRASH COURSE" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="WEB STACK" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TOPIC" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="CRASH COURSE" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2617,20 +2608,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="30.77734375" style="2" customWidth="1"/>
-    <col min="4" max="6" width="80.77734375" style="2" customWidth="1"/>
+    <col min="2" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="6" width="80.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="19.95" customHeight="1">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="19.899999999999999" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2942,20 +2935,20 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>185</v>
+      <c r="B14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>180</v>
@@ -2965,20 +2958,20 @@
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>188</v>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>180</v>
@@ -2988,20 +2981,20 @@
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>191</v>
+      <c r="B16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>180</v>
@@ -3011,20 +3004,20 @@
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>196</v>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>180</v>
@@ -3034,20 +3027,20 @@
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>200</v>
+      <c r="B18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>180</v>
@@ -3057,20 +3050,20 @@
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>204</v>
+      <c r="B19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>180</v>
@@ -3080,20 +3073,20 @@
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>208</v>
+      <c r="B20" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>180</v>
@@ -3103,20 +3096,20 @@
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>213</v>
+      <c r="B21" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>180</v>
@@ -3126,20 +3119,20 @@
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>217</v>
+      <c r="B22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>180</v>
@@ -3149,20 +3142,20 @@
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>221</v>
+      <c r="B23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>180</v>
@@ -3172,20 +3165,20 @@
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>225</v>
+      <c r="B24" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>180</v>
@@ -3196,19 +3189,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>61</v>
+        <v>106</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>180</v>
@@ -3218,20 +3211,20 @@
       <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>67</v>
+      <c r="B26" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>185</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>180</v>
@@ -3241,20 +3234,20 @@
       <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>72</v>
+      <c r="B27" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>180</v>
@@ -3264,20 +3257,20 @@
       <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>76</v>
+      <c r="B28" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>180</v>
@@ -3287,20 +3280,20 @@
       <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>80</v>
+      <c r="B29" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>180</v>
@@ -3310,20 +3303,20 @@
       <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>84</v>
+      <c r="B30" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>200</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>180</v>
@@ -3333,20 +3326,20 @@
       <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>89</v>
+      <c r="B31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>180</v>
@@ -3356,20 +3349,20 @@
       <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>93</v>
+      <c r="B32" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>180</v>
@@ -3379,20 +3372,20 @@
       <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>97</v>
+      <c r="B33" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>180</v>
@@ -3402,20 +3395,20 @@
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>101</v>
+      <c r="B34" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>180</v>
@@ -3425,20 +3418,20 @@
       <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>105</v>
+      <c r="B35" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>180</v>
@@ -3448,20 +3441,20 @@
       <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>109</v>
+      <c r="B36" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="G36" s="4" t="s">
         <v>180</v>
@@ -3824,11 +3817,8 @@
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please choose a valid status from the list: Completed, Partially Completed, or Not Completed." promptTitle="Task Status" prompt="Please select the current status from the list: Completed, Partially Completed, or Not Completed." sqref="G3:G51">
-      <formula1>$I$2:$I$4</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please choose a valid status from the list: Completed, Partially Completed, or Not Completed." promptTitle="Task Status" prompt="Please select the current status from the list: Completed, Partially Completed, or Not Completed." sqref="G2">
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Entry" error="Please choose a valid status from the list: Completed, Partially Completed, or Not Completed." promptTitle="Task Status" prompt="Please select the current status from the list: Completed, Partially Completed, or Not Completed." sqref="G2:G51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$I$2:$I$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -3841,144 +3831,141 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.95" customHeight="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.899999999999999" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A2" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "Git and GitHub")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "MongoDB")</f>
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10" t="s">
+    <row r="4" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "Node.js + Express + MongoDB")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "MongoDB + Mongoose CRUD")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="10" t="s">
+    <row r="6" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "REST API Design + Postman")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "Authentication &amp; Integration")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "HTML")</f>
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "CSS")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "JavaScript")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="10" t="s">
+    <row r="11" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <f>COUNTIF('MERN Stack'!B:B, "React and Rest API integration")</f>
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="9"/>
-    </row>
-    <row r="13" spans="1:3" ht="19.95" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12" t="s">
+    <row r="12" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:3" ht="19.899999999999999" customHeight="1">
+      <c r="B13" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <f>SUM(C2:C12)</f>
         <v>50</v>
       </c>

</xml_diff>